<commit_message>
Removed AI, implemented speedy Zombie
</commit_message>
<xml_diff>
--- a/rapports/Scrum.xlsx
+++ b/rapports/Scrum.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15975" yWindow="-30" windowWidth="22395" windowHeight="18210" tabRatio="858" activeTab="5"/>
+    <workbookView xWindow="15975" yWindow="-30" windowWidth="22395" windowHeight="18210" tabRatio="858" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="146">
   <si>
     <t>Users stories</t>
   </si>
@@ -462,6 +462,9 @@
   </si>
   <si>
     <t>Coder le sable qui est remplacé par de l'eau</t>
+  </si>
+  <si>
+    <t>Coder un déplacement plus rapide du zombie</t>
   </si>
 </sst>
 </file>
@@ -996,11 +999,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="184582144"/>
-        <c:axId val="184583680"/>
+        <c:axId val="154632192"/>
+        <c:axId val="154633728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="184582144"/>
+        <c:axId val="154632192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1038,7 +1041,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="184583680"/>
+        <c:crossAx val="154633728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1046,7 +1049,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="184583680"/>
+        <c:axId val="154633728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1133,7 +1136,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="184582144"/>
+        <c:crossAx val="154632192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1217,7 +1220,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1431,11 +1433,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="184672640"/>
-        <c:axId val="184674176"/>
+        <c:axId val="154734976"/>
+        <c:axId val="154736512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="184672640"/>
+        <c:axId val="154734976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1473,7 +1475,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="184674176"/>
+        <c:crossAx val="154736512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1481,7 +1483,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="184674176"/>
+        <c:axId val="154736512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1534,7 +1536,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1569,7 +1570,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="184672640"/>
+        <c:crossAx val="154734976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1582,7 +1583,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1867,11 +1867,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="185090816"/>
-        <c:axId val="185092352"/>
+        <c:axId val="155157248"/>
+        <c:axId val="155158784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="185090816"/>
+        <c:axId val="155157248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1909,7 +1909,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="185092352"/>
+        <c:crossAx val="155158784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1917,7 +1917,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="185092352"/>
+        <c:axId val="155158784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2004,7 +2004,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="185090816"/>
+        <c:crossAx val="155157248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2088,6 +2088,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2165,19 +2166,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>68</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>58</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>29</c:v>
@@ -2259,22 +2260,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>68</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>56.666666666666664</c:v>
+                  <c:v>51.666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45.333333333333329</c:v>
+                  <c:v>41.333333333333329</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33.999999999999993</c:v>
+                  <c:v>30.999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22.666666666666657</c:v>
+                  <c:v>20.666666666666657</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.333333333333323</c:v>
+                  <c:v>10.333333333333323</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -2301,11 +2302,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="184846976"/>
-        <c:axId val="184861056"/>
+        <c:axId val="154920064"/>
+        <c:axId val="154921600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="184846976"/>
+        <c:axId val="154920064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2343,7 +2344,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="184861056"/>
+        <c:crossAx val="154921600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2351,7 +2352,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="184861056"/>
+        <c:axId val="154921600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -2404,6 +2405,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -2438,7 +2440,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="184846976"/>
+        <c:crossAx val="154920064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2451,6 +2453,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7730,7 +7733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -9666,8 +9669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10102,22 +10105,22 @@
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="17" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="C11" s="13">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D11" s="13">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E11" s="13">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F11" s="13">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G11" s="13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H11" s="13">
         <v>0</v>
@@ -11177,23 +11180,23 @@
       </c>
       <c r="C44" s="5">
         <f>SUM(C3:C37)</f>
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D44" s="5">
         <f t="shared" ref="D44:I44" si="0">SUM(D3:D37)</f>
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E44" s="5">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="F44" s="5">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G44" s="5">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H44" s="5">
         <f t="shared" si="0"/>
@@ -11250,27 +11253,27 @@
       </c>
       <c r="C46" s="5">
         <f>C44</f>
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D46" s="5">
         <f>C46 - C49</f>
-        <v>56.666666666666664</v>
+        <v>51.666666666666664</v>
       </c>
       <c r="E46" s="5">
         <f>D46 - C49</f>
-        <v>45.333333333333329</v>
+        <v>41.333333333333329</v>
       </c>
       <c r="F46" s="5">
         <f>E46 - C49</f>
-        <v>33.999999999999993</v>
+        <v>30.999999999999993</v>
       </c>
       <c r="G46" s="5">
         <f>F46 - C49</f>
-        <v>22.666666666666657</v>
+        <v>20.666666666666657</v>
       </c>
       <c r="H46" s="5">
         <f>G46 - C49</f>
-        <v>11.333333333333323</v>
+        <v>10.333333333333323</v>
       </c>
       <c r="I46" s="5">
         <f>H46 - C49</f>
@@ -11326,7 +11329,7 @@
       </c>
       <c r="C49" s="5">
         <f>SUM(C44)/C48</f>
-        <v>11.333333333333334</v>
+        <v>10.333333333333334</v>
       </c>
       <c r="R49" s="6"/>
       <c r="S49" s="6"/>

</xml_diff>